<commit_message>
Last (but one) tuning up to PVBASE[0][39]. STC: Score of RubiChess-Bitboard-tune10-1 vs RubiChess-Bitboard-ms: 788 - 694 - 735  [0.521] 2217 Elo difference: 14.74 +/- 11.82 SPRT: llr 1.4, lbound -1.39, ubound 1.39 - H1 was accepted
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Testresults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$49</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="91">
   <si>
     <t>Datum</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>155-157-188</t>
+  </si>
+  <si>
+    <t>163-97.240</t>
   </si>
 </sst>
 </file>
@@ -1086,9 +1089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1849,16 +1854,16 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43247</v>
+        <v>43302</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="C26">
-        <v>24466081</v>
+        <v>11336459</v>
       </c>
       <c r="D26" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -1870,10 +1875,10 @@
         <v>500</v>
       </c>
       <c r="H26" s="2">
-        <v>44</v>
+        <v>42.3</v>
       </c>
       <c r="I26" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1881,10 +1886,10 @@
         <v>43247</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C27">
-        <v>8067271</v>
+        <v>24466081</v>
       </c>
       <c r="D27" t="s">
         <v>40</v>
@@ -1899,21 +1904,21 @@
         <v>500</v>
       </c>
       <c r="H27" s="2">
-        <v>45.9</v>
+        <v>44</v>
       </c>
       <c r="I27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43272</v>
+        <v>43247</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C28">
-        <v>9668840</v>
+        <v>8067271</v>
       </c>
       <c r="D28" t="s">
         <v>40</v>
@@ -1928,10 +1933,10 @@
         <v>500</v>
       </c>
       <c r="H28" s="2">
-        <v>51.4</v>
+        <v>45.9</v>
       </c>
       <c r="I28" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1939,10 +1944,10 @@
         <v>43272</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C29">
-        <v>10578627</v>
+        <v>9668840</v>
       </c>
       <c r="D29" t="s">
         <v>40</v>
@@ -1957,21 +1962,21 @@
         <v>500</v>
       </c>
       <c r="H29" s="2">
-        <v>52.5</v>
+        <v>51.4</v>
       </c>
       <c r="I29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43286</v>
+        <v>43272</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C30">
-        <v>48569661</v>
+        <v>10578627</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -1986,21 +1991,21 @@
         <v>500</v>
       </c>
       <c r="H30" s="2">
-        <v>54.4</v>
+        <v>52.5</v>
       </c>
       <c r="I30" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43293</v>
+        <v>43286</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C31">
-        <v>10731388</v>
+        <v>48569661</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
@@ -2015,10 +2020,10 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>62</v>
+        <v>54.4</v>
       </c>
       <c r="I31" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -2026,13 +2031,13 @@
         <v>43293</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C32">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2044,10 +2049,10 @@
         <v>500</v>
       </c>
       <c r="H32" s="2">
-        <v>43.2</v>
+        <v>62</v>
       </c>
       <c r="I32" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -2055,10 +2060,10 @@
         <v>43293</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C33">
-        <v>10731388</v>
+        <v>9824914</v>
       </c>
       <c r="D33" t="s">
         <v>61</v>
@@ -2073,24 +2078,24 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>63.7</v>
+        <v>43.2</v>
       </c>
       <c r="I33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43243</v>
+        <v>43293</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C34">
-        <v>24466081</v>
+        <v>10731388</v>
       </c>
       <c r="D34" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2099,24 +2104,24 @@
         <v>18</v>
       </c>
       <c r="G34">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>35.299999999999997</v>
+        <v>63.7</v>
       </c>
       <c r="I34" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43246</v>
+        <v>43243</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>8067271</v>
+        <v>24466081</v>
       </c>
       <c r="D35" t="s">
         <v>33</v>
@@ -2128,24 +2133,24 @@
         <v>18</v>
       </c>
       <c r="G35">
-        <v>500</v>
+        <v>851</v>
       </c>
       <c r="H35" s="2">
-        <v>38</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I35" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43272</v>
+        <v>43246</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C36">
-        <v>9668840</v>
+        <v>8067271</v>
       </c>
       <c r="D36" t="s">
         <v>33</v>
@@ -2160,10 +2165,10 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>37.299999999999997</v>
+        <v>38</v>
       </c>
       <c r="I36" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
@@ -2171,10 +2176,10 @@
         <v>43272</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C37">
-        <v>10578627</v>
+        <v>9668840</v>
       </c>
       <c r="D37" t="s">
         <v>33</v>
@@ -2189,21 +2194,21 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>42.3</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43286</v>
+        <v>43272</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C38">
-        <v>48569661</v>
+        <v>10578627</v>
       </c>
       <c r="D38" t="s">
         <v>33</v>
@@ -2218,21 +2223,21 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>48.6</v>
+        <v>42.3</v>
       </c>
       <c r="I38" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43293</v>
+        <v>43286</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C39">
-        <v>10731388</v>
+        <v>48569661</v>
       </c>
       <c r="D39" t="s">
         <v>33</v>
@@ -2247,24 +2252,24 @@
         <v>500</v>
       </c>
       <c r="H39" s="2">
-        <v>51.7</v>
+        <v>48.6</v>
       </c>
       <c r="I39" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43295</v>
+        <v>43293</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C40">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2276,21 +2281,21 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>37.1</v>
+        <v>51.7</v>
       </c>
       <c r="I40" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43296</v>
+        <v>43295</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C41">
-        <v>10731388</v>
+        <v>9824914</v>
       </c>
       <c r="D41" t="s">
         <v>77</v>
@@ -2305,24 +2310,24 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>52.6</v>
+        <v>37.1</v>
       </c>
       <c r="I41" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43298</v>
+        <v>43296</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C42">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2334,10 +2339,10 @@
         <v>500</v>
       </c>
       <c r="H42" s="2">
-        <v>50.3</v>
+        <v>52.6</v>
       </c>
       <c r="I42" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -2345,10 +2350,10 @@
         <v>43298</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C43">
-        <v>10731388</v>
+        <v>9824914</v>
       </c>
       <c r="D43" t="s">
         <v>84</v>
@@ -2363,24 +2368,24 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>65.900000000000006</v>
+        <v>50.3</v>
       </c>
       <c r="I43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43243</v>
+        <v>43298</v>
       </c>
       <c r="B44" t="s">
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="C44">
-        <v>3629408</v>
+        <v>10731388</v>
       </c>
       <c r="D44" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2392,10 +2397,10 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>50.4</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="I44" t="s">
-        <v>28</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -2403,10 +2408,10 @@
         <v>43243</v>
       </c>
       <c r="B45" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>1738268</v>
+        <v>3629408</v>
       </c>
       <c r="D45" t="s">
         <v>27</v>
@@ -2418,13 +2423,13 @@
         <v>18</v>
       </c>
       <c r="G45">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>52.1</v>
+        <v>50.4</v>
       </c>
       <c r="I45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -2432,10 +2437,10 @@
         <v>43243</v>
       </c>
       <c r="B46" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C46">
-        <v>24466081</v>
+        <v>1738268</v>
       </c>
       <c r="D46" t="s">
         <v>27</v>
@@ -2447,24 +2452,24 @@
         <v>18</v>
       </c>
       <c r="G46">
-        <v>500</v>
+        <v>753</v>
       </c>
       <c r="H46" s="2">
-        <v>52.6</v>
+        <v>52.1</v>
       </c>
       <c r="I46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43246</v>
+        <v>43243</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C47">
-        <v>8067271</v>
+        <v>24466081</v>
       </c>
       <c r="D47" t="s">
         <v>27</v>
@@ -2479,21 +2484,21 @@
         <v>500</v>
       </c>
       <c r="H47" s="2">
-        <v>57.1</v>
+        <v>52.6</v>
       </c>
       <c r="I47" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43294</v>
+        <v>43246</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C48">
-        <v>10731388</v>
+        <v>8067271</v>
       </c>
       <c r="D48" t="s">
         <v>27</v>
@@ -2508,14 +2513,43 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="I48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>43294</v>
+      </c>
+      <c r="B49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C49">
+        <v>10731388</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49">
+        <v>500</v>
+      </c>
+      <c r="H49" s="2">
         <v>68.900000000000006</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I49" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J48"/>
+  <autoFilter ref="A1:J49"/>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>

<commit_message>
Start new dev cycle.
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Testresults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$53</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="97">
   <si>
     <t>Datum</t>
   </si>
@@ -261,9 +261,6 @@
     <t>183-160-157</t>
   </si>
   <si>
-    <t>109-95-296</t>
-  </si>
-  <si>
     <t>97-142-261</t>
   </si>
   <si>
@@ -295,6 +292,27 @@
   </si>
   <si>
     <t>163-97.240</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>114-145-241</t>
+  </si>
+  <si>
+    <t>4x timeforfeit Devel</t>
+  </si>
+  <si>
+    <t>150-194-156</t>
+  </si>
+  <si>
+    <t>versehentlich nochmal gestartet, deshalb 2x</t>
+  </si>
+  <si>
+    <t>91.147-262</t>
+  </si>
+  <si>
+    <t>174-111-215</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1585,7 +1603,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43293</v>
       </c>
@@ -1614,7 +1632,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43294</v>
       </c>
@@ -1640,10 +1658,10 @@
         <v>33.6</v>
       </c>
       <c r="I18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43295</v>
       </c>
@@ -1672,12 +1690,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43301</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20">
         <v>11336459</v>
@@ -1698,21 +1716,21 @@
         <v>46.7</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43295</v>
+        <v>43317</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C21">
-        <v>10731388</v>
+        <v>11806602</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1724,24 +1742,21 @@
         <v>500</v>
       </c>
       <c r="H21" s="2">
-        <v>36.700000000000003</v>
+        <v>49.4</v>
       </c>
       <c r="I21" t="s">
-        <v>75</v>
-      </c>
-      <c r="J21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43295</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C22">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D22" t="s">
         <v>74</v>
@@ -1756,24 +1771,24 @@
         <v>500</v>
       </c>
       <c r="H22" s="2">
-        <v>25.1</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="J22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43301</v>
+        <v>43295</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="C23">
-        <v>11336459</v>
+        <v>9824914</v>
       </c>
       <c r="D23" t="s">
         <v>74</v>
@@ -1788,224 +1803,236 @@
         <v>500</v>
       </c>
       <c r="H23" s="2">
+        <v>25.1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>80</v>
+      </c>
+      <c r="J23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>43301</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24">
+        <v>11336459</v>
+      </c>
+      <c r="D24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24">
+        <v>500</v>
+      </c>
+      <c r="H24" s="2">
         <v>36.1</v>
       </c>
-      <c r="I23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="I24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25">
+        <v>11806602</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25">
+        <v>500</v>
+      </c>
+      <c r="H25" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="I25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26">
+        <v>11806602</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26">
+        <v>500</v>
+      </c>
+      <c r="H26" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="I26" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" t="s">
+        <v>81</v>
+      </c>
+      <c r="K26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
         <v>43293</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>60</v>
       </c>
-      <c r="C24">
+      <c r="C27">
         <v>9824914</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D27" t="s">
         <v>70</v>
       </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
-        <v>18</v>
-      </c>
-      <c r="G24">
-        <v>500</v>
-      </c>
-      <c r="H24" s="2">
-        <v>31.3</v>
-      </c>
-      <c r="I24" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="E27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>500</v>
+      </c>
+      <c r="H27" s="2">
+        <v>32.9</v>
+      </c>
+      <c r="I27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
         <v>43294</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>63</v>
       </c>
-      <c r="C25">
+      <c r="C28">
         <v>10731388</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>70</v>
       </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25">
-        <v>500</v>
-      </c>
-      <c r="H25" s="2">
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28">
+        <v>500</v>
+      </c>
+      <c r="H28" s="2">
         <v>41.2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>43302</v>
       </c>
-      <c r="B26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26">
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29">
         <v>11336459</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D29" t="s">
         <v>70</v>
       </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26">
-        <v>500</v>
-      </c>
-      <c r="H26" s="2">
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29">
+        <v>500</v>
+      </c>
+      <c r="H29" s="2">
         <v>42.3</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B30" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="C30">
+        <v>11806602</v>
+      </c>
+      <c r="D30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E30" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G30">
+        <v>500</v>
+      </c>
+      <c r="H30" s="2">
+        <v>45.9</v>
+      </c>
+      <c r="I30" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
         <v>43247</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B31" t="s">
         <v>30</v>
       </c>
-      <c r="C27">
+      <c r="C31">
         <v>24466081</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27">
-        <v>500</v>
-      </c>
-      <c r="H27" s="2">
-        <v>44</v>
-      </c>
-      <c r="I27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>43247</v>
-      </c>
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28">
-        <v>8067271</v>
-      </c>
-      <c r="D28" t="s">
-        <v>40</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28">
-        <v>500</v>
-      </c>
-      <c r="H28" s="2">
-        <v>45.9</v>
-      </c>
-      <c r="I28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>43272</v>
-      </c>
-      <c r="B29" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29">
-        <v>9668840</v>
-      </c>
-      <c r="D29" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" t="s">
-        <v>12</v>
-      </c>
-      <c r="F29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G29">
-        <v>500</v>
-      </c>
-      <c r="H29" s="2">
-        <v>51.4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>43272</v>
-      </c>
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30">
-        <v>10578627</v>
-      </c>
-      <c r="D30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30">
-        <v>500</v>
-      </c>
-      <c r="H30" s="2">
-        <v>52.5</v>
-      </c>
-      <c r="I30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>43286</v>
-      </c>
-      <c r="B31" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31">
-        <v>48569661</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
@@ -2020,21 +2047,21 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>54.4</v>
+        <v>44</v>
       </c>
       <c r="I31" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43293</v>
+        <v>43247</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C32">
-        <v>10731388</v>
+        <v>8067271</v>
       </c>
       <c r="D32" t="s">
         <v>40</v>
@@ -2049,24 +2076,24 @@
         <v>500</v>
       </c>
       <c r="H32" s="2">
-        <v>62</v>
+        <v>45.9</v>
       </c>
       <c r="I32" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C33">
-        <v>9824914</v>
+        <v>9668840</v>
       </c>
       <c r="D33" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2078,24 +2105,24 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>43.2</v>
+        <v>51.4</v>
       </c>
       <c r="I33" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C34">
-        <v>10731388</v>
+        <v>10578627</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2107,24 +2134,24 @@
         <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>63.7</v>
+        <v>52.5</v>
       </c>
       <c r="I34" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43243</v>
+        <v>43286</v>
       </c>
       <c r="B35" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C35">
-        <v>24466081</v>
+        <v>48569661</v>
       </c>
       <c r="D35" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2133,27 +2160,27 @@
         <v>18</v>
       </c>
       <c r="G35">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H35" s="2">
-        <v>35.299999999999997</v>
+        <v>54.4</v>
       </c>
       <c r="I35" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43246</v>
+        <v>43293</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>8067271</v>
+        <v>10731388</v>
       </c>
       <c r="D36" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2165,24 +2192,24 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="I36" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43272</v>
+        <v>43293</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>9668840</v>
+        <v>9824914</v>
       </c>
       <c r="D37" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2194,24 +2221,24 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>37.299999999999997</v>
+        <v>43.2</v>
       </c>
       <c r="I37" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43272</v>
+        <v>43293</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C38">
-        <v>10578627</v>
+        <v>10731388</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2223,21 +2250,21 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>42.3</v>
+        <v>63.7</v>
       </c>
       <c r="I38" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43286</v>
+        <v>43243</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C39">
-        <v>48569661</v>
+        <v>24466081</v>
       </c>
       <c r="D39" t="s">
         <v>33</v>
@@ -2249,24 +2276,24 @@
         <v>18</v>
       </c>
       <c r="G39">
-        <v>500</v>
+        <v>851</v>
       </c>
       <c r="H39" s="2">
-        <v>48.6</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I39" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43293</v>
+        <v>43246</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C40">
-        <v>10731388</v>
+        <v>8067271</v>
       </c>
       <c r="D40" t="s">
         <v>33</v>
@@ -2281,24 +2308,24 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>51.7</v>
+        <v>38</v>
       </c>
       <c r="I40" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>9824914</v>
+        <v>9668840</v>
       </c>
       <c r="D41" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2310,24 +2337,24 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>37.1</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I41" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43296</v>
+        <v>43272</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C42">
-        <v>10731388</v>
+        <v>10578627</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2339,24 +2366,24 @@
         <v>500</v>
       </c>
       <c r="H42" s="2">
-        <v>52.6</v>
+        <v>42.3</v>
       </c>
       <c r="I42" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43298</v>
+        <v>43286</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C43">
-        <v>9824914</v>
+        <v>48569661</v>
       </c>
       <c r="D43" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2368,15 +2395,15 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>50.3</v>
+        <v>48.6</v>
       </c>
       <c r="I43" t="s">
-        <v>85</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43298</v>
+        <v>43293</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
@@ -2385,7 +2412,7 @@
         <v>10731388</v>
       </c>
       <c r="D44" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2397,24 +2424,24 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>65.900000000000006</v>
+        <v>51.7</v>
       </c>
       <c r="I44" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43243</v>
+        <v>43295</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C45">
-        <v>3629408</v>
+        <v>9824914</v>
       </c>
       <c r="D45" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2426,24 +2453,24 @@
         <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>50.4</v>
+        <v>37.1</v>
       </c>
       <c r="I45" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43243</v>
+        <v>43296</v>
       </c>
       <c r="B46" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C46">
-        <v>1738268</v>
+        <v>10731388</v>
       </c>
       <c r="D46" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2452,27 +2479,27 @@
         <v>18</v>
       </c>
       <c r="G46">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H46" s="2">
-        <v>52.1</v>
+        <v>52.6</v>
       </c>
       <c r="I46" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43243</v>
+        <v>43298</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C47">
-        <v>24466081</v>
+        <v>9824914</v>
       </c>
       <c r="D47" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2484,24 +2511,24 @@
         <v>500</v>
       </c>
       <c r="H47" s="2">
-        <v>52.6</v>
+        <v>50.3</v>
       </c>
       <c r="I47" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43246</v>
+        <v>43298</v>
       </c>
       <c r="B48" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C48">
-        <v>8067271</v>
+        <v>10731388</v>
       </c>
       <c r="D48" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2513,21 +2540,21 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
-        <v>57.1</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="I48" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43294</v>
+        <v>43243</v>
       </c>
       <c r="B49" t="s">
-        <v>63</v>
+        <v>10</v>
       </c>
       <c r="C49">
-        <v>10731388</v>
+        <v>3629408</v>
       </c>
       <c r="D49" t="s">
         <v>27</v>
@@ -2542,14 +2569,130 @@
         <v>500</v>
       </c>
       <c r="H49" s="2">
+        <v>50.4</v>
+      </c>
+      <c r="I49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50">
+        <v>1738268</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>753</v>
+      </c>
+      <c r="H50" s="2">
+        <v>52.1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B51" t="s">
+        <v>30</v>
+      </c>
+      <c r="C51">
+        <v>24466081</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51">
+        <v>500</v>
+      </c>
+      <c r="H51" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="I51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>43246</v>
+      </c>
+      <c r="B52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52">
+        <v>8067271</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52">
+        <v>500</v>
+      </c>
+      <c r="H52" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="I52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>43294</v>
+      </c>
+      <c r="B53" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53">
+        <v>10731388</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53">
+        <v>500</v>
+      </c>
+      <c r="H53" s="2">
         <v>68.900000000000006</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I53" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J49"/>
+  <autoFilter ref="A1:J53"/>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>

<commit_message>
Updated ChangeLog and testresults.
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Testresults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$59</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="106">
   <si>
     <t>Datum</t>
   </si>
@@ -309,10 +309,37 @@
     <t>versehentlich nochmal gestartet, deshalb 2x</t>
   </si>
   <si>
-    <t>91.147-262</t>
-  </si>
-  <si>
     <t>174-111-215</t>
+  </si>
+  <si>
+    <t>91-147-262</t>
+  </si>
+  <si>
+    <t>MS 10.8.18</t>
+  </si>
+  <si>
+    <t>141-133-226</t>
+  </si>
+  <si>
+    <t>5x timeforfeit Devel</t>
+  </si>
+  <si>
+    <t>186-112-202</t>
+  </si>
+  <si>
+    <t>138 - 165 - 197  [0.473]</t>
+  </si>
+  <si>
+    <t>138-197-165</t>
+  </si>
+  <si>
+    <t>214-118-168</t>
+  </si>
+  <si>
+    <t>207-146-147</t>
+  </si>
+  <si>
+    <t>198-166-136</t>
   </si>
 </sst>
 </file>
@@ -1107,10 +1134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1750,16 +1777,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43295</v>
+        <v>43322</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C22">
-        <v>10731388</v>
+        <v>11528022</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1771,13 +1798,13 @@
         <v>500</v>
       </c>
       <c r="H22" s="2">
-        <v>36.700000000000003</v>
+        <v>47.3</v>
       </c>
       <c r="I22" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
       <c r="J22" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1785,10 +1812,10 @@
         <v>43295</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C23">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D23" t="s">
         <v>74</v>
@@ -1803,24 +1830,24 @@
         <v>500</v>
       </c>
       <c r="H23" s="2">
-        <v>25.1</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43301</v>
+        <v>43295</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C24">
-        <v>11336459</v>
+        <v>9824914</v>
       </c>
       <c r="D24" t="s">
         <v>74</v>
@@ -1835,21 +1862,24 @@
         <v>500</v>
       </c>
       <c r="H24" s="2">
-        <v>36.1</v>
+        <v>25.1</v>
       </c>
       <c r="I24" t="s">
-        <v>87</v>
+        <v>80</v>
+      </c>
+      <c r="J24" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43317</v>
+        <v>43301</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C25">
-        <v>11806602</v>
+        <v>11336459</v>
       </c>
       <c r="D25" t="s">
         <v>74</v>
@@ -1864,13 +1894,10 @@
         <v>500</v>
       </c>
       <c r="H25" s="2">
-        <v>37.299999999999997</v>
+        <v>36.1</v>
       </c>
       <c r="I25" t="s">
-        <v>91</v>
-      </c>
-      <c r="J25" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1902,24 +1929,21 @@
         <v>91</v>
       </c>
       <c r="J26" t="s">
-        <v>81</v>
-      </c>
-      <c r="K26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43293</v>
+        <v>43317</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C27">
-        <v>9824914</v>
+        <v>11806602</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1934,21 +1958,27 @@
         <v>32.9</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>96</v>
+      </c>
+      <c r="J27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K27" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43294</v>
+        <v>43322</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C28">
-        <v>10731388</v>
+        <v>11528022</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -1960,21 +1990,24 @@
         <v>500</v>
       </c>
       <c r="H28" s="2">
-        <v>41.2</v>
+        <v>41.5</v>
       </c>
       <c r="I28" t="s">
-        <v>71</v>
+        <v>98</v>
+      </c>
+      <c r="J28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43302</v>
+        <v>43293</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C29">
-        <v>11336459</v>
+        <v>9824914</v>
       </c>
       <c r="D29" t="s">
         <v>70</v>
@@ -1989,21 +2022,21 @@
         <v>500</v>
       </c>
       <c r="H29" s="2">
-        <v>42.3</v>
+        <v>32.9</v>
       </c>
       <c r="I29" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43317</v>
+        <v>43294</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C30">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D30" t="s">
         <v>70</v>
@@ -2018,24 +2051,24 @@
         <v>500</v>
       </c>
       <c r="H30" s="2">
-        <v>45.9</v>
+        <v>41.2</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43247</v>
+        <v>43302</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C31">
-        <v>24466081</v>
+        <v>11336459</v>
       </c>
       <c r="D31" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2047,24 +2080,24 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>44</v>
+        <v>42.3</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43247</v>
+        <v>43317</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C32">
-        <v>8067271</v>
+        <v>11806602</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2079,21 +2112,21 @@
         <v>45.9</v>
       </c>
       <c r="I32" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>43272</v>
+        <v>43322</v>
       </c>
       <c r="B33" t="s">
-        <v>46</v>
+        <v>97</v>
       </c>
       <c r="C33">
-        <v>9668840</v>
+        <v>11528022</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2105,21 +2138,21 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>51.4</v>
+        <v>48.4</v>
       </c>
       <c r="I33" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43272</v>
+        <v>43247</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C34">
-        <v>10578627</v>
+        <v>24466081</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
@@ -2134,21 +2167,21 @@
         <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>52.5</v>
+        <v>44</v>
       </c>
       <c r="I34" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43286</v>
+        <v>43247</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C35">
-        <v>48569661</v>
+        <v>8067271</v>
       </c>
       <c r="D35" t="s">
         <v>40</v>
@@ -2163,21 +2196,21 @@
         <v>500</v>
       </c>
       <c r="H35" s="2">
-        <v>54.4</v>
+        <v>45.9</v>
       </c>
       <c r="I35" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C36">
-        <v>10731388</v>
+        <v>9668840</v>
       </c>
       <c r="D36" t="s">
         <v>40</v>
@@ -2192,24 +2225,24 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>62</v>
+        <v>51.4</v>
       </c>
       <c r="I36" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B37" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C37">
-        <v>9824914</v>
+        <v>10578627</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2221,24 +2254,24 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>43.2</v>
+        <v>52.5</v>
       </c>
       <c r="I37" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43293</v>
+        <v>43286</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C38">
-        <v>10731388</v>
+        <v>48569661</v>
       </c>
       <c r="D38" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2250,24 +2283,24 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>63.7</v>
+        <v>54.4</v>
       </c>
       <c r="I38" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43243</v>
+        <v>43293</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C39">
-        <v>24466081</v>
+        <v>10731388</v>
       </c>
       <c r="D39" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2276,27 +2309,27 @@
         <v>18</v>
       </c>
       <c r="G39">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H39" s="2">
-        <v>35.299999999999997</v>
+        <v>62</v>
       </c>
       <c r="I39" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43246</v>
+        <v>43293</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C40">
-        <v>8067271</v>
+        <v>9824914</v>
       </c>
       <c r="D40" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2308,24 +2341,24 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>38</v>
+        <v>43.2</v>
       </c>
       <c r="I40" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43272</v>
+        <v>43293</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C41">
-        <v>9668840</v>
+        <v>10731388</v>
       </c>
       <c r="D41" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2337,21 +2370,21 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>37.299999999999997</v>
+        <v>63.7</v>
       </c>
       <c r="I41" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43272</v>
+        <v>43243</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C42">
-        <v>10578627</v>
+        <v>24466081</v>
       </c>
       <c r="D42" t="s">
         <v>33</v>
@@ -2363,24 +2396,24 @@
         <v>18</v>
       </c>
       <c r="G42">
-        <v>500</v>
+        <v>851</v>
       </c>
       <c r="H42" s="2">
-        <v>42.3</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I42" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43286</v>
+        <v>43246</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C43">
-        <v>48569661</v>
+        <v>8067271</v>
       </c>
       <c r="D43" t="s">
         <v>33</v>
@@ -2395,21 +2428,21 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>48.6</v>
+        <v>38</v>
       </c>
       <c r="I43" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C44">
-        <v>10731388</v>
+        <v>9668840</v>
       </c>
       <c r="D44" t="s">
         <v>33</v>
@@ -2424,24 +2457,24 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>51.7</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I44" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B45" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C45">
-        <v>9824914</v>
+        <v>10578627</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2453,24 +2486,24 @@
         <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>37.1</v>
+        <v>42.3</v>
       </c>
       <c r="I45" t="s">
-        <v>82</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43296</v>
+        <v>43286</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C46">
-        <v>10731388</v>
+        <v>48569661</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2482,24 +2515,24 @@
         <v>500</v>
       </c>
       <c r="H46" s="2">
-        <v>52.6</v>
+        <v>48.6</v>
       </c>
       <c r="I46" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43298</v>
+        <v>43293</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C47">
-        <v>9824914</v>
+        <v>10731388</v>
       </c>
       <c r="D47" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2511,24 +2544,24 @@
         <v>500</v>
       </c>
       <c r="H47" s="2">
-        <v>50.3</v>
+        <v>51.7</v>
       </c>
       <c r="I47" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43298</v>
+        <v>43323</v>
       </c>
       <c r="B48" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C48">
-        <v>10731388</v>
+        <v>11528022</v>
       </c>
       <c r="D48" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2540,24 +2573,24 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
-        <v>65.900000000000006</v>
+        <v>54.6</v>
       </c>
       <c r="I48" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43243</v>
+        <v>43295</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C49">
-        <v>3629408</v>
+        <v>9824914</v>
       </c>
       <c r="D49" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2569,24 +2602,24 @@
         <v>500</v>
       </c>
       <c r="H49" s="2">
-        <v>50.4</v>
+        <v>37.1</v>
       </c>
       <c r="I49" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43243</v>
+        <v>43296</v>
       </c>
       <c r="B50" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C50">
-        <v>1738268</v>
+        <v>10731388</v>
       </c>
       <c r="D50" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2595,27 +2628,27 @@
         <v>18</v>
       </c>
       <c r="G50">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H50" s="2">
-        <v>52.1</v>
+        <v>52.6</v>
       </c>
       <c r="I50" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43243</v>
+        <v>43326</v>
       </c>
       <c r="B51" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C51">
-        <v>24466081</v>
+        <v>11528022</v>
       </c>
       <c r="D51" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2627,24 +2660,24 @@
         <v>500</v>
       </c>
       <c r="H51" s="2">
-        <v>52.6</v>
+        <v>56</v>
       </c>
       <c r="I51" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43246</v>
+        <v>43317</v>
       </c>
       <c r="B52" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C52">
-        <v>8067271</v>
+        <v>11806602</v>
       </c>
       <c r="D52" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2656,43 +2689,217 @@
         <v>500</v>
       </c>
       <c r="H52" s="2">
-        <v>57.1</v>
+        <v>56.2</v>
       </c>
       <c r="I52" t="s">
-        <v>36</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
+        <v>43298</v>
+      </c>
+      <c r="B53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53">
+        <v>9824914</v>
+      </c>
+      <c r="D53" t="s">
+        <v>83</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53">
+        <v>500</v>
+      </c>
+      <c r="H53" s="2">
+        <v>50.3</v>
+      </c>
+      <c r="I53" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43298</v>
+      </c>
+      <c r="B54" t="s">
+        <v>63</v>
+      </c>
+      <c r="C54">
+        <v>10731388</v>
+      </c>
+      <c r="D54" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54">
+        <v>500</v>
+      </c>
+      <c r="H54" s="2">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="I54" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B55" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>3629408</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55">
+        <v>500</v>
+      </c>
+      <c r="H55" s="2">
+        <v>50.4</v>
+      </c>
+      <c r="I55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>1738268</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56">
+        <v>753</v>
+      </c>
+      <c r="H56" s="2">
+        <v>52.1</v>
+      </c>
+      <c r="I56" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B57" t="s">
+        <v>30</v>
+      </c>
+      <c r="C57">
+        <v>24466081</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>500</v>
+      </c>
+      <c r="H57" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="I57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43246</v>
+      </c>
+      <c r="B58" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58">
+        <v>8067271</v>
+      </c>
+      <c r="D58" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58">
+        <v>500</v>
+      </c>
+      <c r="H58" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="I58" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
         <v>43294</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B59" t="s">
         <v>63</v>
       </c>
-      <c r="C53">
+      <c r="C59">
         <v>10731388</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D59" t="s">
         <v>27</v>
       </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53">
-        <v>500</v>
-      </c>
-      <c r="H53" s="2">
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59">
+        <v>500</v>
+      </c>
+      <c r="H59" s="2">
         <v>68.900000000000006</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I59" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J53"/>
+  <autoFilter ref="A1:J59"/>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>

<commit_message>
Updates Testresults and Bench.
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\RubiChess\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Testresults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$65</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="114">
   <si>
     <t>Datum</t>
   </si>
@@ -327,9 +327,6 @@
     <t>186-112-202</t>
   </si>
   <si>
-    <t>138 - 165 - 197  [0.473]</t>
-  </si>
-  <si>
     <t>138-197-165</t>
   </si>
   <si>
@@ -340,6 +337,33 @@
   </si>
   <si>
     <t>198-166-136</t>
+  </si>
+  <si>
+    <t>115-157-228</t>
+  </si>
+  <si>
+    <t>9x timeforfeit Devel</t>
+  </si>
+  <si>
+    <t>171-169-160</t>
+  </si>
+  <si>
+    <t>179-122-199</t>
+  </si>
+  <si>
+    <t>240-123-137</t>
+  </si>
+  <si>
+    <t>MS 19.8.18</t>
+  </si>
+  <si>
+    <t>366-80-54</t>
+  </si>
+  <si>
+    <t>349-98-53</t>
+  </si>
+  <si>
+    <t>weils der letzte Test gegen Bumble ist(?) und das vorherige Ergebnis etwas enttäuschend war</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="J52" sqref="J52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1661,16 +1685,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43294</v>
+        <v>43331</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="C18">
-        <v>9824914</v>
-      </c>
-      <c r="D18" t="s">
-        <v>72</v>
+        <v>14367150</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1682,24 +1703,21 @@
         <v>500</v>
       </c>
       <c r="H18" s="2">
-        <v>33.6</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="I18" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43295</v>
+        <v>43331</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C19">
-        <v>10731388</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
+        <v>14367150</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1711,21 +1729,27 @@
         <v>500</v>
       </c>
       <c r="H19" s="2">
-        <v>43.4</v>
+        <v>81.2</v>
       </c>
       <c r="I19" t="s">
-        <v>73</v>
+        <v>111</v>
+      </c>
+      <c r="J19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43301</v>
+        <v>43294</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="C20">
-        <v>11336459</v>
+        <v>9824914</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -1740,21 +1764,21 @@
         <v>500</v>
       </c>
       <c r="H20" s="2">
-        <v>46.7</v>
+        <v>33.6</v>
       </c>
       <c r="I20" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43317</v>
+        <v>43295</v>
       </c>
       <c r="B21" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C21">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
@@ -1769,21 +1793,21 @@
         <v>500</v>
       </c>
       <c r="H21" s="2">
-        <v>49.4</v>
+        <v>43.4</v>
       </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43322</v>
+        <v>43301</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C22">
-        <v>11528022</v>
+        <v>11336459</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
@@ -1798,27 +1822,24 @@
         <v>500</v>
       </c>
       <c r="H22" s="2">
-        <v>47.3</v>
+        <v>46.7</v>
       </c>
       <c r="I22" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43295</v>
+        <v>43317</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C23">
-        <v>10731388</v>
+        <v>11806602</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
@@ -1830,27 +1851,24 @@
         <v>500</v>
       </c>
       <c r="H23" s="2">
-        <v>36.700000000000003</v>
+        <v>49.4</v>
       </c>
       <c r="I23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J23" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43295</v>
+        <v>43322</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C24">
-        <v>9824914</v>
+        <v>11528022</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1862,27 +1880,24 @@
         <v>500</v>
       </c>
       <c r="H24" s="2">
-        <v>25.1</v>
+        <v>47.3</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
-      </c>
-      <c r="J24" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43301</v>
+        <v>43330</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="C25">
-        <v>11336459</v>
+        <v>14367150</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1894,21 +1909,21 @@
         <v>500</v>
       </c>
       <c r="H25" s="2">
-        <v>36.1</v>
+        <v>51.1</v>
       </c>
       <c r="I25" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43317</v>
+        <v>43295</v>
       </c>
       <c r="B26" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C26">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D26" t="s">
         <v>74</v>
@@ -1923,24 +1938,24 @@
         <v>500</v>
       </c>
       <c r="H26" s="2">
-        <v>37.299999999999997</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="I26" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="J26" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43317</v>
+        <v>43295</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C27">
-        <v>11806602</v>
+        <v>9824914</v>
       </c>
       <c r="D27" t="s">
         <v>74</v>
@@ -1955,27 +1970,24 @@
         <v>500</v>
       </c>
       <c r="H27" s="2">
-        <v>32.9</v>
+        <v>25.1</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="J27" t="s">
         <v>81</v>
       </c>
-      <c r="K27" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43322</v>
+        <v>43301</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C28">
-        <v>11528022</v>
+        <v>11336459</v>
       </c>
       <c r="D28" t="s">
         <v>74</v>
@@ -1990,27 +2002,24 @@
         <v>500</v>
       </c>
       <c r="H28" s="2">
-        <v>41.5</v>
+        <v>36.1</v>
       </c>
       <c r="I28" t="s">
-        <v>98</v>
-      </c>
-      <c r="J28" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43293</v>
+        <v>43317</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="C29">
-        <v>9824914</v>
+        <v>11806602</v>
       </c>
       <c r="D29" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2022,24 +2031,27 @@
         <v>500</v>
       </c>
       <c r="H29" s="2">
-        <v>32.9</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I29" t="s">
-        <v>96</v>
+        <v>91</v>
+      </c>
+      <c r="J29" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43294</v>
+        <v>43317</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C30">
-        <v>10731388</v>
+        <v>11806602</v>
       </c>
       <c r="D30" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2051,24 +2063,30 @@
         <v>500</v>
       </c>
       <c r="H30" s="2">
-        <v>41.2</v>
+        <v>32.9</v>
       </c>
       <c r="I30" t="s">
-        <v>71</v>
+        <v>96</v>
+      </c>
+      <c r="J30" t="s">
+        <v>81</v>
+      </c>
+      <c r="K30" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43302</v>
+        <v>43322</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C31">
-        <v>11336459</v>
+        <v>11528022</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2080,24 +2098,27 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>42.3</v>
+        <v>41.5</v>
       </c>
       <c r="I31" t="s">
-        <v>89</v>
+        <v>98</v>
+      </c>
+      <c r="J31" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43317</v>
+        <v>43330</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="C32">
-        <v>11806602</v>
+        <v>14367150</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2109,21 +2130,24 @@
         <v>500</v>
       </c>
       <c r="H32" s="2">
-        <v>45.9</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="I32" t="s">
-        <v>95</v>
+        <v>105</v>
+      </c>
+      <c r="J32" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>43322</v>
+        <v>43293</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C33">
-        <v>11528022</v>
+        <v>9824914</v>
       </c>
       <c r="D33" t="s">
         <v>70</v>
@@ -2138,24 +2162,24 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>48.4</v>
+        <v>32.9</v>
       </c>
       <c r="I33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43247</v>
+        <v>43294</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C34">
-        <v>24466081</v>
+        <v>10731388</v>
       </c>
       <c r="D34" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2167,24 +2191,24 @@
         <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>44</v>
+        <v>41.2</v>
       </c>
       <c r="I34" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43247</v>
+        <v>43302</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C35">
-        <v>8067271</v>
+        <v>11336459</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2196,24 +2220,24 @@
         <v>500</v>
       </c>
       <c r="H35" s="2">
-        <v>45.9</v>
+        <v>42.3</v>
       </c>
       <c r="I35" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43272</v>
+        <v>43317</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C36">
-        <v>9668840</v>
+        <v>11806602</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2225,24 +2249,24 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>51.4</v>
+        <v>45.9</v>
       </c>
       <c r="I36" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43272</v>
+        <v>43322</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="C37">
-        <v>10578627</v>
+        <v>11528022</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2254,24 +2278,24 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>52.5</v>
+        <v>48.4</v>
       </c>
       <c r="I37" t="s">
-        <v>56</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43286</v>
+        <v>43330</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="C38">
-        <v>48569661</v>
+        <v>14367150</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E38" t="s">
         <v>12</v>
@@ -2283,21 +2307,21 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>54.4</v>
+        <v>48</v>
       </c>
       <c r="I38" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43293</v>
+        <v>43247</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C39">
-        <v>10731388</v>
+        <v>24466081</v>
       </c>
       <c r="D39" t="s">
         <v>40</v>
@@ -2312,24 +2336,24 @@
         <v>500</v>
       </c>
       <c r="H39" s="2">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43293</v>
+        <v>43247</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C40">
-        <v>9824914</v>
+        <v>8067271</v>
       </c>
       <c r="D40" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2341,24 +2365,24 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>43.2</v>
+        <v>45.9</v>
       </c>
       <c r="I40" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43293</v>
+        <v>43272</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C41">
-        <v>10731388</v>
+        <v>9668840</v>
       </c>
       <c r="D41" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2370,24 +2394,24 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>63.7</v>
+        <v>51.4</v>
       </c>
       <c r="I41" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43243</v>
+        <v>43272</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C42">
-        <v>24466081</v>
+        <v>10578627</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2396,27 +2420,27 @@
         <v>18</v>
       </c>
       <c r="G42">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H42" s="2">
-        <v>35.299999999999997</v>
+        <v>52.5</v>
       </c>
       <c r="I42" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43246</v>
+        <v>43286</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C43">
-        <v>8067271</v>
+        <v>48569661</v>
       </c>
       <c r="D43" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2428,24 +2452,24 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>38</v>
+        <v>54.4</v>
       </c>
       <c r="I43" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43272</v>
+        <v>43293</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C44">
-        <v>9668840</v>
+        <v>10731388</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2457,24 +2481,24 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>37.299999999999997</v>
+        <v>62</v>
       </c>
       <c r="I44" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43272</v>
+        <v>43293</v>
       </c>
       <c r="B45" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C45">
-        <v>10578627</v>
+        <v>9824914</v>
       </c>
       <c r="D45" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2486,24 +2510,24 @@
         <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>42.3</v>
+        <v>43.2</v>
       </c>
       <c r="I45" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43286</v>
+        <v>43293</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C46">
-        <v>48569661</v>
+        <v>10731388</v>
       </c>
       <c r="D46" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2515,21 +2539,21 @@
         <v>500</v>
       </c>
       <c r="H46" s="2">
-        <v>48.6</v>
+        <v>63.7</v>
       </c>
       <c r="I46" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43293</v>
+        <v>43243</v>
       </c>
       <c r="B47" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="C47">
-        <v>10731388</v>
+        <v>24466081</v>
       </c>
       <c r="D47" t="s">
         <v>33</v>
@@ -2541,24 +2565,24 @@
         <v>18</v>
       </c>
       <c r="G47">
-        <v>500</v>
+        <v>851</v>
       </c>
       <c r="H47" s="2">
-        <v>51.7</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I47" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43323</v>
+        <v>43246</v>
       </c>
       <c r="B48" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="C48">
-        <v>11528022</v>
+        <v>8067271</v>
       </c>
       <c r="D48" t="s">
         <v>33</v>
@@ -2573,24 +2597,24 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
-        <v>54.6</v>
+        <v>38</v>
       </c>
       <c r="I48" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C49">
-        <v>9824914</v>
+        <v>9668840</v>
       </c>
       <c r="D49" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2602,24 +2626,24 @@
         <v>500</v>
       </c>
       <c r="H49" s="2">
-        <v>37.1</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I49" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>43296</v>
+        <v>43272</v>
       </c>
       <c r="B50" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C50">
-        <v>10731388</v>
+        <v>10578627</v>
       </c>
       <c r="D50" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E50" t="s">
         <v>12</v>
@@ -2631,24 +2655,24 @@
         <v>500</v>
       </c>
       <c r="H50" s="2">
-        <v>52.6</v>
+        <v>42.3</v>
       </c>
       <c r="I50" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>43326</v>
+        <v>43286</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C51">
-        <v>11528022</v>
+        <v>48569661</v>
       </c>
       <c r="D51" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -2660,24 +2684,24 @@
         <v>500</v>
       </c>
       <c r="H51" s="2">
-        <v>56</v>
+        <v>48.6</v>
       </c>
       <c r="I51" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43317</v>
+        <v>43293</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C52">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2689,24 +2713,24 @@
         <v>500</v>
       </c>
       <c r="H52" s="2">
-        <v>56.2</v>
+        <v>51.7</v>
       </c>
       <c r="I52" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43298</v>
+        <v>43323</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="C53">
-        <v>9824914</v>
+        <v>11528022</v>
       </c>
       <c r="D53" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2718,24 +2742,24 @@
         <v>500</v>
       </c>
       <c r="H53" s="2">
-        <v>50.3</v>
+        <v>54.6</v>
       </c>
       <c r="I53" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>43298</v>
+        <v>43330</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C54">
-        <v>10731388</v>
+        <v>14367150</v>
       </c>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2747,24 +2771,24 @@
         <v>500</v>
       </c>
       <c r="H54" s="2">
-        <v>65.900000000000006</v>
+        <v>60.3</v>
       </c>
       <c r="I54" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>43243</v>
+        <v>43295</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="C55">
-        <v>3629408</v>
+        <v>9824914</v>
       </c>
       <c r="D55" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2776,24 +2800,24 @@
         <v>500</v>
       </c>
       <c r="H55" s="2">
-        <v>50.4</v>
+        <v>37.1</v>
       </c>
       <c r="I55" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>43243</v>
+        <v>43296</v>
       </c>
       <c r="B56" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="C56">
-        <v>1738268</v>
+        <v>10731388</v>
       </c>
       <c r="D56" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2802,27 +2826,27 @@
         <v>18</v>
       </c>
       <c r="G56">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H56" s="2">
-        <v>52.1</v>
+        <v>52.6</v>
       </c>
       <c r="I56" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>43243</v>
+        <v>43326</v>
       </c>
       <c r="B57" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="C57">
-        <v>24466081</v>
+        <v>11528022</v>
       </c>
       <c r="D57" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2834,24 +2858,24 @@
         <v>500</v>
       </c>
       <c r="H57" s="2">
-        <v>52.6</v>
+        <v>56</v>
       </c>
       <c r="I57" t="s">
-        <v>32</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>43246</v>
+        <v>43317</v>
       </c>
       <c r="B58" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="C58">
-        <v>8067271</v>
+        <v>11806602</v>
       </c>
       <c r="D58" t="s">
-        <v>27</v>
+        <v>77</v>
       </c>
       <c r="E58" t="s">
         <v>12</v>
@@ -2863,43 +2887,217 @@
         <v>500</v>
       </c>
       <c r="H58" s="2">
-        <v>57.1</v>
+        <v>56.2</v>
       </c>
       <c r="I58" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
+        <v>43298</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59">
+        <v>9824914</v>
+      </c>
+      <c r="D59" t="s">
+        <v>83</v>
+      </c>
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59">
+        <v>500</v>
+      </c>
+      <c r="H59" s="2">
+        <v>50.3</v>
+      </c>
+      <c r="I59" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>43298</v>
+      </c>
+      <c r="B60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60">
+        <v>10731388</v>
+      </c>
+      <c r="D60" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60">
+        <v>500</v>
+      </c>
+      <c r="H60" s="2">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="I60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B61" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>3629408</v>
+      </c>
+      <c r="D61" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61">
+        <v>500</v>
+      </c>
+      <c r="H61" s="2">
+        <v>50.4</v>
+      </c>
+      <c r="I61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B62" t="s">
+        <v>15</v>
+      </c>
+      <c r="C62">
+        <v>1738268</v>
+      </c>
+      <c r="D62" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62">
+        <v>753</v>
+      </c>
+      <c r="H62" s="2">
+        <v>52.1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>43243</v>
+      </c>
+      <c r="B63" t="s">
+        <v>30</v>
+      </c>
+      <c r="C63">
+        <v>24466081</v>
+      </c>
+      <c r="D63" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63">
+        <v>500</v>
+      </c>
+      <c r="H63" s="2">
+        <v>52.6</v>
+      </c>
+      <c r="I63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>43246</v>
+      </c>
+      <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64">
+        <v>8067271</v>
+      </c>
+      <c r="D64" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64">
+        <v>500</v>
+      </c>
+      <c r="H64" s="2">
+        <v>57.1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
         <v>43294</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B65" t="s">
         <v>63</v>
       </c>
-      <c r="C59">
+      <c r="C65">
         <v>10731388</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D65" t="s">
         <v>27</v>
       </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59">
-        <v>500</v>
-      </c>
-      <c r="H59" s="2">
+      <c r="E65" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65">
+        <v>500</v>
+      </c>
+      <c r="H65" s="2">
         <v>68.900000000000006</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I65" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J59"/>
+  <autoFilter ref="A1:J65"/>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>

<commit_message>
Updated bench and testresult.
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\RubiChess\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="116">
   <si>
     <t>Datum</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t>weils der letzte Test gegen Bumble ist(?) und das vorherige Ergebnis etwas enttäuschend war</t>
+  </si>
+  <si>
+    <t>MS 17.9.18</t>
+  </si>
+  <si>
+    <t>142-152-206</t>
   </si>
 </sst>
 </file>
@@ -1158,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1203,16 +1209,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43248</v>
+        <v>43237</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>24466081</v>
+        <v>11248014</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1224,111 +1230,117 @@
         <v>500</v>
       </c>
       <c r="H2" s="2">
-        <v>45.9</v>
+        <v>50.6</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43248</v>
+        <v>43241</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>8067271</v>
+        <v>3629408</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H3" s="2">
-        <v>48.3</v>
+        <v>58.1</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43271</v>
+        <v>43241</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>9668840</v>
+        <v>1738268</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H4" s="2">
-        <v>52.3</v>
+        <v>57.1</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43271</v>
+        <v>43242</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>10578627</v>
+        <v>3629408</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>500</v>
       </c>
       <c r="H5" s="2">
-        <v>54.9</v>
+        <v>56.4</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43294</v>
+        <v>43242</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>10731388</v>
+        <v>1723931</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1337,24 +1349,24 @@
         <v>18</v>
       </c>
       <c r="G6">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="H6" s="2">
-        <v>61.3</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43237</v>
+        <v>43242</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>11248014</v>
+        <v>1791160</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1369,24 +1381,21 @@
         <v>500</v>
       </c>
       <c r="H7" s="2">
-        <v>50.6</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43241</v>
+        <v>43243</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>3629408</v>
+        <v>24466081</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1395,53 +1404,53 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H8" s="2">
-        <v>58.1</v>
+        <v>60.6</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43241</v>
+        <v>43243</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>1738268</v>
+        <v>24466081</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>501</v>
+        <v>851</v>
       </c>
       <c r="H9" s="2">
-        <v>57.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1450,7 +1459,7 @@
         <v>3629408</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1462,24 +1471,24 @@
         <v>500</v>
       </c>
       <c r="H10" s="2">
-        <v>56.4</v>
+        <v>50.4</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>1723931</v>
+        <v>1738268</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1488,27 +1497,27 @@
         <v>18</v>
       </c>
       <c r="G11">
-        <v>450</v>
+        <v>753</v>
       </c>
       <c r="H11" s="2">
-        <v>54</v>
+        <v>52.1</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>1791160</v>
+        <v>24466081</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1520,21 +1529,21 @@
         <v>500</v>
       </c>
       <c r="H12" s="2">
-        <v>57</v>
+        <v>52.6</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43243</v>
+        <v>43246</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>24466081</v>
+        <v>8067271</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1549,10 +1558,10 @@
         <v>500</v>
       </c>
       <c r="H13" s="2">
-        <v>60.6</v>
+        <v>58.6</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
@@ -1569,7 +1578,7 @@
         <v>8067271</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1581,27 +1590,24 @@
         <v>500</v>
       </c>
       <c r="H14" s="2">
-        <v>58.6</v>
+        <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>43271</v>
+        <v>43246</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C15">
-        <v>9668840</v>
+        <v>8067271</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1613,59 +1619,53 @@
         <v>500</v>
       </c>
       <c r="H15" s="2">
-        <v>64.900000000000006</v>
+        <v>57.1</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>43271</v>
+        <v>43247</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>10578627</v>
+        <v>24466081</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <v>500</v>
       </c>
       <c r="H16" s="2">
-        <v>68.599999999999994</v>
+        <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>43293</v>
+        <v>43247</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>10731388</v>
+        <v>8067271</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1677,21 +1677,24 @@
         <v>500</v>
       </c>
       <c r="H17" s="2">
-        <v>77.2</v>
+        <v>45.9</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43331</v>
+        <v>43248</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>14367150</v>
+        <v>24466081</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1703,21 +1706,24 @@
         <v>500</v>
       </c>
       <c r="H18" s="2">
-        <v>79.599999999999994</v>
+        <v>45.9</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43331</v>
+        <v>43248</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C19">
-        <v>14367150</v>
+        <v>8067271</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1729,13 +1735,10 @@
         <v>500</v>
       </c>
       <c r="H19" s="2">
-        <v>81.2</v>
+        <v>48.3</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="K19" t="s">
         <v>113</v>
@@ -1743,16 +1746,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43294</v>
+        <v>43271</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>9824914</v>
+        <v>9668840</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1764,53 +1767,53 @@
         <v>500</v>
       </c>
       <c r="H20" s="2">
-        <v>33.6</v>
+        <v>52.3</v>
       </c>
       <c r="I20" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43295</v>
+        <v>43271</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>10731388</v>
+        <v>10578627</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G21">
         <v>500</v>
       </c>
       <c r="H21" s="2">
-        <v>43.4</v>
+        <v>54.9</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43301</v>
+        <v>43271</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>11336459</v>
+        <v>9668840</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1822,53 +1825,59 @@
         <v>500</v>
       </c>
       <c r="H22" s="2">
-        <v>46.7</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="I22" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43317</v>
+        <v>43271</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>11806602</v>
+        <v>10578627</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G23">
         <v>500</v>
       </c>
       <c r="H23" s="2">
-        <v>49.4</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>51</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43322</v>
+        <v>43272</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="C24">
-        <v>11528022</v>
+        <v>9668840</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1880,24 +1889,24 @@
         <v>500</v>
       </c>
       <c r="H24" s="2">
-        <v>47.3</v>
+        <v>51.4</v>
       </c>
       <c r="I24" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43330</v>
+        <v>43272</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>14367150</v>
+        <v>10578627</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1909,24 +1918,24 @@
         <v>500</v>
       </c>
       <c r="H25" s="2">
-        <v>51.1</v>
+        <v>52.5</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>10731388</v>
+        <v>9668840</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -1938,27 +1947,24 @@
         <v>500</v>
       </c>
       <c r="H26" s="2">
-        <v>36.700000000000003</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>9824914</v>
+        <v>10578627</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1970,27 +1976,24 @@
         <v>500</v>
       </c>
       <c r="H27" s="2">
-        <v>25.1</v>
+        <v>42.3</v>
       </c>
       <c r="I27" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43301</v>
+        <v>43286</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C28">
-        <v>11336459</v>
+        <v>48569661</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2002,24 +2005,24 @@
         <v>500</v>
       </c>
       <c r="H28" s="2">
-        <v>36.1</v>
+        <v>54.4</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43317</v>
+        <v>43286</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="C29">
-        <v>11806602</v>
+        <v>48569661</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2031,27 +2034,24 @@
         <v>500</v>
       </c>
       <c r="H29" s="2">
-        <v>37.299999999999997</v>
+        <v>48.6</v>
       </c>
       <c r="I29" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43317</v>
+        <v>43293</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C30">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2063,13 +2063,10 @@
         <v>500</v>
       </c>
       <c r="H30" s="2">
-        <v>32.9</v>
+        <v>77.2</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="K30" t="s">
         <v>94</v>
@@ -2077,16 +2074,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43322</v>
+        <v>43293</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C31">
-        <v>11528022</v>
+        <v>9824914</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2098,27 +2095,24 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>41.5</v>
+        <v>32.9</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43330</v>
+        <v>43293</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="C32">
-        <v>14367150</v>
+        <v>10731388</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2130,16 +2124,13 @@
         <v>500</v>
       </c>
       <c r="H32" s="2">
-        <v>38.700000000000003</v>
+        <v>62</v>
       </c>
       <c r="I32" t="s">
-        <v>105</v>
-      </c>
-      <c r="J32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43293</v>
       </c>
@@ -2150,7 +2141,7 @@
         <v>9824914</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2162,15 +2153,15 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>32.9</v>
+        <v>43.2</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43294</v>
+        <v>43293</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
@@ -2179,7 +2170,7 @@
         <v>10731388</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2191,24 +2182,24 @@
         <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>41.2</v>
+        <v>63.7</v>
       </c>
       <c r="I34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43302</v>
+        <v>43293</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C35">
-        <v>11336459</v>
+        <v>10731388</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2220,24 +2211,24 @@
         <v>500</v>
       </c>
       <c r="H35" s="2">
-        <v>42.3</v>
+        <v>51.7</v>
       </c>
       <c r="I35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43317</v>
+        <v>43294</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2249,24 +2240,24 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>45.9</v>
+        <v>61.3</v>
       </c>
       <c r="I36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43322</v>
+        <v>43294</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>11528022</v>
+        <v>9824914</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2278,21 +2269,21 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>48.4</v>
+        <v>33.6</v>
       </c>
       <c r="I37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43330</v>
+        <v>43294</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="C38">
-        <v>14367150</v>
+        <v>10731388</v>
       </c>
       <c r="D38" t="s">
         <v>70</v>
@@ -2307,24 +2298,24 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>48</v>
+        <v>41.2</v>
       </c>
       <c r="I38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43247</v>
+        <v>43294</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C39">
-        <v>24466081</v>
+        <v>10731388</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2336,24 +2327,24 @@
         <v>500</v>
       </c>
       <c r="H39" s="2">
-        <v>44</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="I39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43247</v>
+        <v>43295</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C40">
-        <v>8067271</v>
+        <v>10731388</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2365,24 +2356,24 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>45.9</v>
+        <v>43.4</v>
       </c>
       <c r="I40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43272</v>
+        <v>43295</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C41">
-        <v>9668840</v>
+        <v>10731388</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2394,24 +2385,27 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>51.4</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="I41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="J41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43272</v>
+        <v>43295</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C42">
-        <v>10578627</v>
+        <v>9824914</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2423,24 +2417,27 @@
         <v>500</v>
       </c>
       <c r="H42" s="2">
-        <v>52.5</v>
+        <v>25.1</v>
       </c>
       <c r="I42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="J42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43286</v>
+        <v>43295</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C43">
-        <v>48569661</v>
+        <v>9824914</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2452,15 +2449,15 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>54.4</v>
+        <v>37.1</v>
       </c>
       <c r="I43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43293</v>
+        <v>43296</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
@@ -2469,7 +2466,7 @@
         <v>10731388</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2481,15 +2478,15 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>62</v>
+        <v>52.6</v>
       </c>
       <c r="I44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43293</v>
+        <v>43298</v>
       </c>
       <c r="B45" t="s">
         <v>60</v>
@@ -2498,7 +2495,7 @@
         <v>9824914</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2510,15 +2507,15 @@
         <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>43.2</v>
+        <v>50.3</v>
       </c>
       <c r="I45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43293</v>
+        <v>43298</v>
       </c>
       <c r="B46" t="s">
         <v>63</v>
@@ -2527,7 +2524,7 @@
         <v>10731388</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2539,24 +2536,24 @@
         <v>500</v>
       </c>
       <c r="H46" s="2">
-        <v>63.7</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="I46" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43243</v>
+        <v>43301</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C47">
-        <v>24466081</v>
+        <v>11336459</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2565,27 +2562,27 @@
         <v>18</v>
       </c>
       <c r="G47">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H47" s="2">
-        <v>35.299999999999997</v>
+        <v>46.7</v>
       </c>
       <c r="I47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43246</v>
+        <v>43301</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C48">
-        <v>8067271</v>
+        <v>11336459</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2597,24 +2594,24 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
-        <v>38</v>
+        <v>36.1</v>
       </c>
       <c r="I48" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43272</v>
+        <v>43302</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C49">
-        <v>9668840</v>
+        <v>11336459</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2626,82 +2623,85 @@
         <v>500</v>
       </c>
       <c r="H49" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50">
+        <v>11806602</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>500</v>
+      </c>
+      <c r="H50" s="2">
+        <v>49.4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51">
+        <v>11806602</v>
+      </c>
+      <c r="D51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51">
+        <v>500</v>
+      </c>
+      <c r="H51" s="2">
         <v>37.299999999999997</v>
       </c>
-      <c r="I49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>43272</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50">
-        <v>10578627</v>
-      </c>
-      <c r="D50" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50">
-        <v>500</v>
-      </c>
-      <c r="H50" s="2">
-        <v>42.3</v>
-      </c>
-      <c r="I50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>43286</v>
-      </c>
-      <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51">
-        <v>48569661</v>
-      </c>
-      <c r="D51" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51">
-        <v>500</v>
-      </c>
-      <c r="H51" s="2">
-        <v>48.6</v>
-      </c>
       <c r="I51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="J51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43293</v>
+        <v>43317</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C52">
-        <v>10731388</v>
+        <v>11806602</v>
       </c>
       <c r="D52" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2713,82 +2713,85 @@
         <v>500</v>
       </c>
       <c r="H52" s="2">
-        <v>51.7</v>
+        <v>32.9</v>
       </c>
       <c r="I52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43323</v>
+        <v>43317</v>
       </c>
       <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53">
+        <v>11806602</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53">
+        <v>500</v>
+      </c>
+      <c r="H53" s="2">
+        <v>45.9</v>
+      </c>
+      <c r="I53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54">
+        <v>11806602</v>
+      </c>
+      <c r="D54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54">
+        <v>500</v>
+      </c>
+      <c r="H54" s="2">
+        <v>56.2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>43322</v>
+      </c>
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="C53">
+      <c r="C55">
         <v>11528022</v>
       </c>
-      <c r="D53" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53">
-        <v>500</v>
-      </c>
-      <c r="H53" s="2">
-        <v>54.6</v>
-      </c>
-      <c r="I53" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>43330</v>
-      </c>
-      <c r="B54" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54">
-        <v>14367150</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54">
-        <v>500</v>
-      </c>
-      <c r="H54" s="2">
-        <v>60.3</v>
-      </c>
-      <c r="I54" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>43295</v>
-      </c>
-      <c r="B55" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55">
-        <v>9824914</v>
-      </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2800,24 +2803,24 @@
         <v>500</v>
       </c>
       <c r="H55" s="2">
-        <v>37.1</v>
+        <v>47.3</v>
       </c>
       <c r="I55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>43296</v>
+        <v>43322</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C56">
-        <v>10731388</v>
+        <v>11528022</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2829,15 +2832,18 @@
         <v>500</v>
       </c>
       <c r="H56" s="2">
-        <v>52.6</v>
+        <v>41.5</v>
       </c>
       <c r="I56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>43326</v>
+        <v>43322</v>
       </c>
       <c r="B57" t="s">
         <v>97</v>
@@ -2846,94 +2852,94 @@
         <v>11528022</v>
       </c>
       <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>500</v>
+      </c>
+      <c r="H57" s="2">
+        <v>48.4</v>
+      </c>
+      <c r="I57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43323</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58">
+        <v>11528022</v>
+      </c>
+      <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58">
+        <v>500</v>
+      </c>
+      <c r="H58" s="2">
+        <v>54.6</v>
+      </c>
+      <c r="I58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43326</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59">
+        <v>11528022</v>
+      </c>
+      <c r="D59" t="s">
         <v>77</v>
       </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57">
-        <v>500</v>
-      </c>
-      <c r="H57" s="2">
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59">
+        <v>500</v>
+      </c>
+      <c r="H59" s="2">
         <v>56</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I59" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>43317</v>
-      </c>
-      <c r="B58" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58">
-        <v>11806602</v>
-      </c>
-      <c r="D58" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58">
-        <v>500</v>
-      </c>
-      <c r="H58" s="2">
-        <v>56.2</v>
-      </c>
-      <c r="I58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>43298</v>
-      </c>
-      <c r="B59" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59">
-        <v>9824914</v>
-      </c>
-      <c r="D59" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59">
-        <v>500</v>
-      </c>
-      <c r="H59" s="2">
-        <v>50.3</v>
-      </c>
-      <c r="I59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>43298</v>
+        <v>43330</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C60">
-        <v>10731388</v>
+        <v>14367150</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -2945,24 +2951,24 @@
         <v>500</v>
       </c>
       <c r="H60" s="2">
-        <v>65.900000000000006</v>
+        <v>51.1</v>
       </c>
       <c r="I60" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C61">
-        <v>3629408</v>
+        <v>14367150</v>
       </c>
       <c r="D61" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -2974,24 +2980,27 @@
         <v>500</v>
       </c>
       <c r="H61" s="2">
-        <v>50.4</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="I61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="J61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="C62">
-        <v>1738268</v>
+        <v>14367150</v>
       </c>
       <c r="D62" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -3000,27 +3009,27 @@
         <v>18</v>
       </c>
       <c r="G62">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H62" s="2">
-        <v>52.1</v>
+        <v>48</v>
       </c>
       <c r="I62" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C63">
-        <v>24466081</v>
+        <v>14367150</v>
       </c>
       <c r="D63" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -3032,24 +3041,24 @@
         <v>500</v>
       </c>
       <c r="H63" s="2">
-        <v>52.6</v>
+        <v>60.3</v>
       </c>
       <c r="I63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>43246</v>
+        <v>43331</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="C64">
-        <v>8067271</v>
+        <v>14367150</v>
       </c>
       <c r="D64" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -3061,24 +3070,24 @@
         <v>500</v>
       </c>
       <c r="H64" s="2">
-        <v>57.1</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="I64" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>43294</v>
+        <v>43331</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C65">
-        <v>10731388</v>
+        <v>14367150</v>
       </c>
       <c r="D65" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -3090,14 +3099,53 @@
         <v>500</v>
       </c>
       <c r="H65" s="2">
-        <v>68.900000000000006</v>
+        <v>81.2</v>
       </c>
       <c r="I65" t="s">
-        <v>69</v>
+        <v>111</v>
+      </c>
+      <c r="J65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43360</v>
+      </c>
+      <c r="B66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66">
+        <v>12788821</v>
+      </c>
+      <c r="D66" t="s">
+        <v>74</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66">
+        <v>500</v>
+      </c>
+      <c r="H66" s="2">
+        <v>43.6</v>
+      </c>
+      <c r="I66" t="s">
+        <v>115</v>
+      </c>
+      <c r="J66" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J65"/>
+  <autoFilter ref="A1:J65">
+    <sortState ref="A2:J65">
+      <sortCondition ref="A1:A65"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>

<commit_message>
Removed test for != PAWN as this is always true now. Added test results.
</commit_message>
<xml_diff>
--- a/Tests/Testresults.xlsx
+++ b/Tests/Testresults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Lokale_Daten_ungesichert\Entwicklung\GitHub\RubiChess\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Testresults" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Testresults!$A$1:$J$68</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="118">
   <si>
     <t>Datum</t>
   </si>
@@ -364,6 +364,18 @@
   </si>
   <si>
     <t>weils der letzte Test gegen Bumble ist(?) und das vorherige Ergebnis etwas enttäuschend war</t>
+  </si>
+  <si>
+    <t>MS 17.9.18</t>
+  </si>
+  <si>
+    <t>142-152-206</t>
+  </si>
+  <si>
+    <t>213-116-171</t>
+  </si>
+  <si>
+    <t>209-166-125</t>
   </si>
 </sst>
 </file>
@@ -1158,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="J68" sqref="J68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1203,16 +1215,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43248</v>
+        <v>43237</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C2">
-        <v>24466081</v>
+        <v>11248014</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -1224,111 +1236,117 @@
         <v>500</v>
       </c>
       <c r="H2" s="2">
-        <v>45.9</v>
+        <v>50.6</v>
       </c>
       <c r="I2" t="s">
-        <v>44</v>
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43248</v>
+        <v>43241</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>8067271</v>
+        <v>3629408</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G3">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H3" s="2">
-        <v>48.3</v>
+        <v>58.1</v>
       </c>
       <c r="I3" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43271</v>
+        <v>43241</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>9668840</v>
+        <v>1738268</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G4">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H4" s="2">
-        <v>52.3</v>
+        <v>57.1</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43271</v>
+        <v>43242</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>10578627</v>
+        <v>3629408</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>500</v>
       </c>
       <c r="H5" s="2">
-        <v>54.9</v>
+        <v>56.4</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>43294</v>
+        <v>43242</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C6">
-        <v>10731388</v>
+        <v>1723931</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1337,24 +1355,24 @@
         <v>18</v>
       </c>
       <c r="G6">
-        <v>500</v>
+        <v>450</v>
       </c>
       <c r="H6" s="2">
-        <v>61.3</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43237</v>
+        <v>43242</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>11248014</v>
+        <v>1791160</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -1369,24 +1387,21 @@
         <v>500</v>
       </c>
       <c r="H7" s="2">
-        <v>50.6</v>
+        <v>57</v>
       </c>
       <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43241</v>
+        <v>43243</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C8">
-        <v>3629408</v>
+        <v>24466081</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -1395,53 +1410,53 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G8">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H8" s="2">
-        <v>58.1</v>
+        <v>60.6</v>
       </c>
       <c r="I8" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="J8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43241</v>
+        <v>43243</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C9">
-        <v>1738268</v>
+        <v>24466081</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G9">
-        <v>501</v>
+        <v>851</v>
       </c>
       <c r="H9" s="2">
-        <v>57.1</v>
+        <v>35.299999999999997</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1450,7 +1465,7 @@
         <v>3629408</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>12</v>
@@ -1462,24 +1477,24 @@
         <v>500</v>
       </c>
       <c r="H10" s="2">
-        <v>56.4</v>
+        <v>50.4</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>1723931</v>
+        <v>1738268</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1488,27 +1503,27 @@
         <v>18</v>
       </c>
       <c r="G11">
-        <v>450</v>
+        <v>753</v>
       </c>
       <c r="H11" s="2">
-        <v>54</v>
+        <v>52.1</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>43242</v>
+        <v>43243</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C12">
-        <v>1791160</v>
+        <v>24466081</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -1520,21 +1535,21 @@
         <v>500</v>
       </c>
       <c r="H12" s="2">
-        <v>57</v>
+        <v>52.6</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>43243</v>
+        <v>43246</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C13">
-        <v>24466081</v>
+        <v>8067271</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -1549,10 +1564,10 @@
         <v>500</v>
       </c>
       <c r="H13" s="2">
-        <v>60.6</v>
+        <v>58.6</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
@@ -1569,7 +1584,7 @@
         <v>8067271</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -1581,27 +1596,24 @@
         <v>500</v>
       </c>
       <c r="H14" s="2">
-        <v>58.6</v>
+        <v>38</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J14" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>43271</v>
+        <v>43246</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C15">
-        <v>9668840</v>
+        <v>8067271</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -1613,59 +1625,53 @@
         <v>500</v>
       </c>
       <c r="H15" s="2">
-        <v>64.900000000000006</v>
+        <v>57.1</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>43271</v>
+        <v>43247</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C16">
-        <v>10578627</v>
+        <v>24466081</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <v>500</v>
       </c>
       <c r="H16" s="2">
-        <v>68.599999999999994</v>
+        <v>44</v>
       </c>
       <c r="I16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J16" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>43293</v>
+        <v>43247</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>10731388</v>
+        <v>8067271</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1677,21 +1683,24 @@
         <v>500</v>
       </c>
       <c r="H17" s="2">
-        <v>77.2</v>
+        <v>45.9</v>
       </c>
       <c r="I17" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43331</v>
+        <v>43248</v>
       </c>
       <c r="B18" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>14367150</v>
+        <v>24466081</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1703,21 +1712,24 @@
         <v>500</v>
       </c>
       <c r="H18" s="2">
-        <v>79.599999999999994</v>
+        <v>45.9</v>
       </c>
       <c r="I18" t="s">
-        <v>112</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>43331</v>
+        <v>43248</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="C19">
-        <v>14367150</v>
+        <v>8067271</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1729,13 +1741,10 @@
         <v>500</v>
       </c>
       <c r="H19" s="2">
-        <v>81.2</v>
+        <v>48.3</v>
       </c>
       <c r="I19" t="s">
-        <v>111</v>
-      </c>
-      <c r="J19" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="K19" t="s">
         <v>113</v>
@@ -1743,16 +1752,16 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>43294</v>
+        <v>43271</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C20">
-        <v>9824914</v>
+        <v>9668840</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1764,53 +1773,53 @@
         <v>500</v>
       </c>
       <c r="H20" s="2">
-        <v>33.6</v>
+        <v>52.3</v>
       </c>
       <c r="I20" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>43295</v>
+        <v>43271</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>10731388</v>
+        <v>10578627</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G21">
         <v>500</v>
       </c>
       <c r="H21" s="2">
-        <v>43.4</v>
+        <v>54.9</v>
       </c>
       <c r="I21" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>43301</v>
+        <v>43271</v>
       </c>
       <c r="B22" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C22">
-        <v>11336459</v>
+        <v>9668840</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -1822,53 +1831,59 @@
         <v>500</v>
       </c>
       <c r="H22" s="2">
-        <v>46.7</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="I22" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="J22" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>43317</v>
+        <v>43271</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="C23">
-        <v>11806602</v>
+        <v>10578627</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
         <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G23">
         <v>500</v>
       </c>
       <c r="H23" s="2">
-        <v>49.4</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>51</v>
+      </c>
+      <c r="J23" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>43322</v>
+        <v>43272</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="C24">
-        <v>11528022</v>
+        <v>9668840</v>
       </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -1880,24 +1895,24 @@
         <v>500</v>
       </c>
       <c r="H24" s="2">
-        <v>47.3</v>
+        <v>51.4</v>
       </c>
       <c r="I24" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>43330</v>
+        <v>43272</v>
       </c>
       <c r="B25" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C25">
-        <v>14367150</v>
+        <v>10578627</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
@@ -1909,24 +1924,24 @@
         <v>500</v>
       </c>
       <c r="H25" s="2">
-        <v>51.1</v>
+        <v>52.5</v>
       </c>
       <c r="I25" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C26">
-        <v>10731388</v>
+        <v>9668840</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>
@@ -1938,27 +1953,24 @@
         <v>500</v>
       </c>
       <c r="H26" s="2">
-        <v>36.700000000000003</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="I26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J26" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>43295</v>
+        <v>43272</v>
       </c>
       <c r="B27" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>9824914</v>
+        <v>10578627</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
         <v>12</v>
@@ -1970,27 +1982,24 @@
         <v>500</v>
       </c>
       <c r="H27" s="2">
-        <v>25.1</v>
+        <v>42.3</v>
       </c>
       <c r="I27" t="s">
-        <v>80</v>
-      </c>
-      <c r="J27" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>43301</v>
+        <v>43286</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C28">
-        <v>11336459</v>
+        <v>48569661</v>
       </c>
       <c r="D28" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2002,24 +2011,24 @@
         <v>500</v>
       </c>
       <c r="H28" s="2">
-        <v>36.1</v>
+        <v>54.4</v>
       </c>
       <c r="I28" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>43317</v>
+        <v>43286</v>
       </c>
       <c r="B29" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="C29">
-        <v>11806602</v>
+        <v>48569661</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2031,27 +2040,24 @@
         <v>500</v>
       </c>
       <c r="H29" s="2">
-        <v>37.299999999999997</v>
+        <v>48.6</v>
       </c>
       <c r="I29" t="s">
-        <v>91</v>
-      </c>
-      <c r="J29" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>43317</v>
+        <v>43293</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C30">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
         <v>12</v>
@@ -2063,13 +2069,10 @@
         <v>500</v>
       </c>
       <c r="H30" s="2">
-        <v>32.9</v>
+        <v>77.2</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="K30" t="s">
         <v>94</v>
@@ -2077,16 +2080,16 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>43322</v>
+        <v>43293</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C31">
-        <v>11528022</v>
+        <v>9824914</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
@@ -2098,27 +2101,24 @@
         <v>500</v>
       </c>
       <c r="H31" s="2">
-        <v>41.5</v>
+        <v>32.9</v>
       </c>
       <c r="I31" t="s">
-        <v>98</v>
-      </c>
-      <c r="J31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>43330</v>
+        <v>43293</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="C32">
-        <v>14367150</v>
+        <v>10731388</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
         <v>12</v>
@@ -2130,16 +2130,13 @@
         <v>500</v>
       </c>
       <c r="H32" s="2">
-        <v>38.700000000000003</v>
+        <v>62</v>
       </c>
       <c r="I32" t="s">
-        <v>105</v>
-      </c>
-      <c r="J32" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43293</v>
       </c>
@@ -2150,7 +2147,7 @@
         <v>9824914</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E33" t="s">
         <v>12</v>
@@ -2162,15 +2159,15 @@
         <v>500</v>
       </c>
       <c r="H33" s="2">
-        <v>32.9</v>
+        <v>43.2</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>43294</v>
+        <v>43293</v>
       </c>
       <c r="B34" t="s">
         <v>63</v>
@@ -2179,7 +2176,7 @@
         <v>10731388</v>
       </c>
       <c r="D34" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E34" t="s">
         <v>12</v>
@@ -2191,24 +2188,24 @@
         <v>500</v>
       </c>
       <c r="H34" s="2">
-        <v>41.2</v>
+        <v>63.7</v>
       </c>
       <c r="I34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>43302</v>
+        <v>43293</v>
       </c>
       <c r="B35" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C35">
-        <v>11336459</v>
+        <v>10731388</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -2220,24 +2217,24 @@
         <v>500</v>
       </c>
       <c r="H35" s="2">
-        <v>42.3</v>
+        <v>51.7</v>
       </c>
       <c r="I35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>43317</v>
+        <v>43294</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>11806602</v>
+        <v>10731388</v>
       </c>
       <c r="D36" t="s">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="E36" t="s">
         <v>12</v>
@@ -2249,24 +2246,24 @@
         <v>500</v>
       </c>
       <c r="H36" s="2">
-        <v>45.9</v>
+        <v>61.3</v>
       </c>
       <c r="I36" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>43322</v>
+        <v>43294</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="C37">
-        <v>11528022</v>
+        <v>9824914</v>
       </c>
       <c r="D37" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E37" t="s">
         <v>12</v>
@@ -2278,21 +2275,21 @@
         <v>500</v>
       </c>
       <c r="H37" s="2">
-        <v>48.4</v>
+        <v>33.6</v>
       </c>
       <c r="I37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>43330</v>
+        <v>43294</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>63</v>
       </c>
       <c r="C38">
-        <v>14367150</v>
+        <v>10731388</v>
       </c>
       <c r="D38" t="s">
         <v>70</v>
@@ -2307,24 +2304,24 @@
         <v>500</v>
       </c>
       <c r="H38" s="2">
-        <v>48</v>
+        <v>41.2</v>
       </c>
       <c r="I38" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>43247</v>
+        <v>43294</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C39">
-        <v>24466081</v>
+        <v>10731388</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E39" t="s">
         <v>12</v>
@@ -2336,24 +2333,24 @@
         <v>500</v>
       </c>
       <c r="H39" s="2">
-        <v>44</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="I39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>43247</v>
+        <v>43295</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="C40">
-        <v>8067271</v>
+        <v>10731388</v>
       </c>
       <c r="D40" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -2365,24 +2362,24 @@
         <v>500</v>
       </c>
       <c r="H40" s="2">
-        <v>45.9</v>
+        <v>43.4</v>
       </c>
       <c r="I40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>43272</v>
+        <v>43295</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C41">
-        <v>9668840</v>
+        <v>10731388</v>
       </c>
       <c r="D41" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E41" t="s">
         <v>12</v>
@@ -2394,24 +2391,27 @@
         <v>500</v>
       </c>
       <c r="H41" s="2">
-        <v>51.4</v>
+        <v>36.700000000000003</v>
       </c>
       <c r="I41" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="J41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>43272</v>
+        <v>43295</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C42">
-        <v>10578627</v>
+        <v>9824914</v>
       </c>
       <c r="D42" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -2423,24 +2423,27 @@
         <v>500</v>
       </c>
       <c r="H42" s="2">
-        <v>52.5</v>
+        <v>25.1</v>
       </c>
       <c r="I42" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="J42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>43286</v>
+        <v>43295</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C43">
-        <v>48569661</v>
+        <v>9824914</v>
       </c>
       <c r="D43" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
@@ -2452,15 +2455,15 @@
         <v>500</v>
       </c>
       <c r="H43" s="2">
-        <v>54.4</v>
+        <v>37.1</v>
       </c>
       <c r="I43" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>43293</v>
+        <v>43296</v>
       </c>
       <c r="B44" t="s">
         <v>63</v>
@@ -2469,7 +2472,7 @@
         <v>10731388</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="E44" t="s">
         <v>12</v>
@@ -2481,15 +2484,15 @@
         <v>500</v>
       </c>
       <c r="H44" s="2">
-        <v>62</v>
+        <v>52.6</v>
       </c>
       <c r="I44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43293</v>
+        <v>43298</v>
       </c>
       <c r="B45" t="s">
         <v>60</v>
@@ -2498,7 +2501,7 @@
         <v>9824914</v>
       </c>
       <c r="D45" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -2510,15 +2513,15 @@
         <v>500</v>
       </c>
       <c r="H45" s="2">
-        <v>43.2</v>
+        <v>50.3</v>
       </c>
       <c r="I45" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>43293</v>
+        <v>43298</v>
       </c>
       <c r="B46" t="s">
         <v>63</v>
@@ -2527,7 +2530,7 @@
         <v>10731388</v>
       </c>
       <c r="D46" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -2539,24 +2542,24 @@
         <v>500</v>
       </c>
       <c r="H46" s="2">
-        <v>63.7</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="I46" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>43243</v>
+        <v>43301</v>
       </c>
       <c r="B47" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="C47">
-        <v>24466081</v>
+        <v>11336459</v>
       </c>
       <c r="D47" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -2565,27 +2568,27 @@
         <v>18</v>
       </c>
       <c r="G47">
-        <v>851</v>
+        <v>500</v>
       </c>
       <c r="H47" s="2">
-        <v>35.299999999999997</v>
+        <v>46.7</v>
       </c>
       <c r="I47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>43246</v>
+        <v>43301</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C48">
-        <v>8067271</v>
+        <v>11336459</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -2597,24 +2600,24 @@
         <v>500</v>
       </c>
       <c r="H48" s="2">
-        <v>38</v>
+        <v>36.1</v>
       </c>
       <c r="I48" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>43272</v>
+        <v>43302</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="C49">
-        <v>9668840</v>
+        <v>11336459</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -2626,82 +2629,85 @@
         <v>500</v>
       </c>
       <c r="H49" s="2">
+        <v>42.3</v>
+      </c>
+      <c r="I49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50">
+        <v>11806602</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50">
+        <v>500</v>
+      </c>
+      <c r="H50" s="2">
+        <v>49.4</v>
+      </c>
+      <c r="I50" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51">
+        <v>11806602</v>
+      </c>
+      <c r="D51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51">
+        <v>500</v>
+      </c>
+      <c r="H51" s="2">
         <v>37.299999999999997</v>
       </c>
-      <c r="I49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>43272</v>
-      </c>
-      <c r="B50" t="s">
-        <v>50</v>
-      </c>
-      <c r="C50">
-        <v>10578627</v>
-      </c>
-      <c r="D50" t="s">
-        <v>33</v>
-      </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50">
-        <v>500</v>
-      </c>
-      <c r="H50" s="2">
-        <v>42.3</v>
-      </c>
-      <c r="I50" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>43286</v>
-      </c>
-      <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C51">
-        <v>48569661</v>
-      </c>
-      <c r="D51" t="s">
-        <v>33</v>
-      </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
-      <c r="G51">
-        <v>500</v>
-      </c>
-      <c r="H51" s="2">
-        <v>48.6</v>
-      </c>
       <c r="I51" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="J51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>43293</v>
+        <v>43317</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C52">
-        <v>10731388</v>
+        <v>11806602</v>
       </c>
       <c r="D52" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -2713,82 +2719,85 @@
         <v>500</v>
       </c>
       <c r="H52" s="2">
-        <v>51.7</v>
+        <v>32.9</v>
       </c>
       <c r="I52" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="J52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>43323</v>
+        <v>43317</v>
       </c>
       <c r="B53" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53">
+        <v>11806602</v>
+      </c>
+      <c r="D53" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53">
+        <v>500</v>
+      </c>
+      <c r="H53" s="2">
+        <v>45.9</v>
+      </c>
+      <c r="I53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43317</v>
+      </c>
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54">
+        <v>11806602</v>
+      </c>
+      <c r="D54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G54">
+        <v>500</v>
+      </c>
+      <c r="H54" s="2">
+        <v>56.2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>43322</v>
+      </c>
+      <c r="B55" t="s">
         <v>97</v>
       </c>
-      <c r="C53">
+      <c r="C55">
         <v>11528022</v>
       </c>
-      <c r="D53" t="s">
-        <v>33</v>
-      </c>
-      <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" t="s">
-        <v>18</v>
-      </c>
-      <c r="G53">
-        <v>500</v>
-      </c>
-      <c r="H53" s="2">
-        <v>54.6</v>
-      </c>
-      <c r="I53" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>43330</v>
-      </c>
-      <c r="B54" t="s">
-        <v>110</v>
-      </c>
-      <c r="C54">
-        <v>14367150</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>12</v>
-      </c>
-      <c r="F54" t="s">
-        <v>18</v>
-      </c>
-      <c r="G54">
-        <v>500</v>
-      </c>
-      <c r="H54" s="2">
-        <v>60.3</v>
-      </c>
-      <c r="I54" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>43295</v>
-      </c>
-      <c r="B55" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55">
-        <v>9824914</v>
-      </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2800,24 +2809,24 @@
         <v>500</v>
       </c>
       <c r="H55" s="2">
-        <v>37.1</v>
+        <v>47.3</v>
       </c>
       <c r="I55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>43296</v>
+        <v>43322</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C56">
-        <v>10731388</v>
+        <v>11528022</v>
       </c>
       <c r="D56" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2829,15 +2838,18 @@
         <v>500</v>
       </c>
       <c r="H56" s="2">
-        <v>52.6</v>
+        <v>41.5</v>
       </c>
       <c r="I56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="J56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>43326</v>
+        <v>43322</v>
       </c>
       <c r="B57" t="s">
         <v>97</v>
@@ -2846,94 +2858,94 @@
         <v>11528022</v>
       </c>
       <c r="D57" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>18</v>
+      </c>
+      <c r="G57">
+        <v>500</v>
+      </c>
+      <c r="H57" s="2">
+        <v>48.4</v>
+      </c>
+      <c r="I57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43323</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58">
+        <v>11528022</v>
+      </c>
+      <c r="D58" t="s">
+        <v>33</v>
+      </c>
+      <c r="E58" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58">
+        <v>500</v>
+      </c>
+      <c r="H58" s="2">
+        <v>54.6</v>
+      </c>
+      <c r="I58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43326</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59">
+        <v>11528022</v>
+      </c>
+      <c r="D59" t="s">
         <v>77</v>
       </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57">
-        <v>500</v>
-      </c>
-      <c r="H57" s="2">
+      <c r="E59" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59">
+        <v>500</v>
+      </c>
+      <c r="H59" s="2">
         <v>56</v>
       </c>
-      <c r="I57" t="s">
+      <c r="I59" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>43317</v>
-      </c>
-      <c r="B58" t="s">
-        <v>90</v>
-      </c>
-      <c r="C58">
-        <v>11806602</v>
-      </c>
-      <c r="D58" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58">
-        <v>500</v>
-      </c>
-      <c r="H58" s="2">
-        <v>56.2</v>
-      </c>
-      <c r="I58" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>43298</v>
-      </c>
-      <c r="B59" t="s">
-        <v>60</v>
-      </c>
-      <c r="C59">
-        <v>9824914</v>
-      </c>
-      <c r="D59" t="s">
-        <v>83</v>
-      </c>
-      <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59">
-        <v>500</v>
-      </c>
-      <c r="H59" s="2">
-        <v>50.3</v>
-      </c>
-      <c r="I59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>43298</v>
+        <v>43330</v>
       </c>
       <c r="B60" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C60">
-        <v>10731388</v>
+        <v>14367150</v>
       </c>
       <c r="D60" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="E60" t="s">
         <v>12</v>
@@ -2945,24 +2957,24 @@
         <v>500</v>
       </c>
       <c r="H60" s="2">
-        <v>65.900000000000006</v>
+        <v>51.1</v>
       </c>
       <c r="I60" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="C61">
-        <v>3629408</v>
+        <v>14367150</v>
       </c>
       <c r="D61" t="s">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="E61" t="s">
         <v>12</v>
@@ -2974,24 +2986,27 @@
         <v>500</v>
       </c>
       <c r="H61" s="2">
-        <v>50.4</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="I61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="J61" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="C62">
-        <v>1738268</v>
+        <v>14367150</v>
       </c>
       <c r="D62" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -3000,27 +3015,27 @@
         <v>18</v>
       </c>
       <c r="G62">
-        <v>753</v>
+        <v>500</v>
       </c>
       <c r="H62" s="2">
-        <v>52.1</v>
+        <v>48</v>
       </c>
       <c r="I62" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>43243</v>
+        <v>43330</v>
       </c>
       <c r="B63" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="C63">
-        <v>24466081</v>
+        <v>14367150</v>
       </c>
       <c r="D63" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -3032,24 +3047,24 @@
         <v>500</v>
       </c>
       <c r="H63" s="2">
-        <v>52.6</v>
+        <v>60.3</v>
       </c>
       <c r="I63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>43246</v>
+        <v>43331</v>
       </c>
       <c r="B64" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="C64">
-        <v>8067271</v>
+        <v>14367150</v>
       </c>
       <c r="D64" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -3061,24 +3076,24 @@
         <v>500</v>
       </c>
       <c r="H64" s="2">
-        <v>57.1</v>
+        <v>79.599999999999994</v>
       </c>
       <c r="I64" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>43294</v>
+        <v>43331</v>
       </c>
       <c r="B65" t="s">
-        <v>63</v>
+        <v>110</v>
       </c>
       <c r="C65">
-        <v>10731388</v>
+        <v>14367150</v>
       </c>
       <c r="D65" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -3090,14 +3105,111 @@
         <v>500</v>
       </c>
       <c r="H65" s="2">
-        <v>68.900000000000006</v>
+        <v>81.2</v>
       </c>
       <c r="I65" t="s">
-        <v>69</v>
+        <v>111</v>
+      </c>
+      <c r="J65" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43360</v>
+      </c>
+      <c r="B66" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66">
+        <v>12788821</v>
+      </c>
+      <c r="D66" t="s">
+        <v>74</v>
+      </c>
+      <c r="E66" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66">
+        <v>500</v>
+      </c>
+      <c r="H66" s="2">
+        <v>43.6</v>
+      </c>
+      <c r="I66" t="s">
+        <v>115</v>
+      </c>
+      <c r="J66" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>43360</v>
+      </c>
+      <c r="B67" t="s">
+        <v>114</v>
+      </c>
+      <c r="C67">
+        <v>12788821</v>
+      </c>
+      <c r="D67" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67">
+        <v>500</v>
+      </c>
+      <c r="H67" s="2">
+        <v>54.2</v>
+      </c>
+      <c r="I67" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43360</v>
+      </c>
+      <c r="B68" t="s">
+        <v>114</v>
+      </c>
+      <c r="C68">
+        <v>12788821</v>
+      </c>
+      <c r="D68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68">
+        <v>500</v>
+      </c>
+      <c r="H68" s="2">
+        <v>58.4</v>
+      </c>
+      <c r="I68" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J65"/>
+  <autoFilter ref="A1:J68">
+    <sortState ref="A2:J65">
+      <sortCondition ref="A1:A65"/>
+    </sortState>
+  </autoFilter>
   <sortState ref="A2:J48">
     <sortCondition ref="D2:D48"/>
     <sortCondition ref="A2:A48"/>

</xml_diff>